<commit_message>
Ajout doc word pour PHPDoc
Modif fichier ficheDevoir pour classes
</commit_message>
<xml_diff>
--- a/EtapesDuDevoir.xlsx
+++ b/EtapesDuDevoir.xlsx
@@ -17,12 +17,12 @@
   <definedNames>
     <definedName name="ListeNoms">"[$#REF !.$B$1:.$B$2]"</definedName>
   </definedNames>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Sujet</t>
   </si>
@@ -175,8 +175,11 @@
     <t>Formulaire de modification d’un téléphone</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">-Documentation du code (norme </t>
+    <t>Lien pour supprimer un contact à partir de la liste (prévoir de demander la confirmation)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fichier zip à envoyer par mail à </t>
     </r>
     <r>
       <rPr>
@@ -185,7 +188,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>PhpDoc</t>
+      <t>benoit@fuleran.net</t>
     </r>
     <r>
       <rPr>
@@ -194,32 +197,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>)  dossier « httpdocs » avec les sources PHP de l’application</t>
-    </r>
-  </si>
-  <si>
-    <t>Lien pour supprimer un contact à partir de la liste (prévoir de demander la confirmation)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fichier zip à envoyer par mail à </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>benoit@fuleran.net</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve"> (avec le nom des binomes)</t>
     </r>
   </si>
@@ -252,6 +229,27 @@
   </si>
   <si>
     <t>Export d’une fiche individuelle sous forme d’un fichier au format vcard</t>
+  </si>
+  <si>
+    <t>Classes :</t>
+  </si>
+  <si>
+    <t>CollectionContact</t>
+  </si>
+  <si>
+    <t>Contact (nom, prénom, société, adresse, date de naissance, commentaire)</t>
+  </si>
+  <si>
+    <t>Adresse(NuméroDeRue,NomDeRue,codePostal,pays)</t>
+  </si>
+  <si>
+    <t>Téléphone(international,professionnel, fixe, portable, fax)</t>
+  </si>
+  <si>
+    <t>CollectionTéléphone</t>
+  </si>
+  <si>
+    <t>Documentation du code (norme PhpDoc)  dossier  httpdocs avec les sources PHP de l'application</t>
   </si>
 </sst>
 </file>
@@ -261,7 +259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-40C];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-40C]"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +329,12 @@
     <font>
       <sz val="15"/>
       <color rgb="FFFF3333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -402,7 +406,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -443,11 +447,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -779,19 +789,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55.375" customWidth="1"/>
-    <col min="2" max="2" width="51.875" customWidth="1"/>
+    <col min="2" max="2" width="57.375" customWidth="1"/>
     <col min="3" max="3" width="26.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
-    <col min="5" max="5" width="42.375" customWidth="1"/>
+    <col min="4" max="4" width="28.375" customWidth="1"/>
+    <col min="5" max="5" width="78.125" customWidth="1"/>
     <col min="6" max="6" width="41.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,7 +824,7 @@
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -830,7 +840,7 @@
       <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
@@ -844,7 +854,7 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
@@ -856,7 +866,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="34.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -868,7 +878,7 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="35.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
@@ -880,63 +890,63 @@
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="10"/>
       <c r="E7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14"/>
+      <c r="B8" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F7" s="11"/>
-    </row>
-    <row r="8" spans="1:6" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="10"/>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="10"/>
       <c r="E9" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="10"/>
       <c r="E10" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="10"/>
@@ -945,33 +955,56 @@
     </row>
     <row r="12" spans="1:6" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="14"/>
+      <c r="E13" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A8"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39409448818897641" bottom="0.39409448818897641" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Répartition des tâches OK
</commit_message>
<xml_diff>
--- a/EtapesDuDevoir.xlsx
+++ b/EtapesDuDevoir.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Sujet</t>
   </si>
@@ -237,19 +237,73 @@
     <t>CollectionContact</t>
   </si>
   <si>
-    <t>Contact (nom, prénom, société, adresse, date de naissance, commentaire)</t>
-  </si>
-  <si>
-    <t>Adresse(NuméroDeRue,NomDeRue,codePostal,pays)</t>
-  </si>
-  <si>
-    <t>Téléphone(international,professionnel, fixe, portable, fax)</t>
-  </si>
-  <si>
     <t>CollectionTéléphone</t>
   </si>
   <si>
     <t>Documentation du code (norme PhpDoc)  dossier  httpdocs avec les sources PHP de l'application</t>
+  </si>
+  <si>
+    <t>AccessDonnees</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Contact</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (nom, prénom, société, adresse, date de naissance, commentaire)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Adresse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(NuméroDeRue,NomDeRue,codePostal,pays)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF002060"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Téléphone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(international,professionnel, fixe, portable, fax)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -259,7 +313,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;[$€-40C];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-40C]"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,12 +369,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF3333"/>
       <name val="Arial"/>
@@ -333,13 +381,56 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="4" tint="-0.499984740745262"/>
+      <b/>
+      <sz val="22"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="5" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,12 +445,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCC99FF"/>
-        <bgColor rgb="FFCC99FF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF9999FF"/>
         <bgColor rgb="FF9999FF"/>
       </patternFill>
@@ -368,6 +453,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF8080"/>
         <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -406,7 +503,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -417,9 +514,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -435,28 +529,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -789,16 +892,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55.375" customWidth="1"/>
-    <col min="2" max="2" width="57.375" customWidth="1"/>
+    <col min="2" max="2" width="59.5" customWidth="1"/>
     <col min="3" max="3" width="26.125" customWidth="1"/>
     <col min="4" max="4" width="28.375" customWidth="1"/>
     <col min="5" max="5" width="78.125" customWidth="1"/>
@@ -812,187 +915,217 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="34.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="6" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="35.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="13"/>
+      <c r="B6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="11"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="6" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" ht="40.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="6" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:6" ht="37.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="12"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="12"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E14" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
+      <c r="C13" s="5"/>
+      <c r="D13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E15" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E18" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E19" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E20" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="E21" s="19" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E16" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E17" s="17" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>